<commit_message>
changed MP time limit and corrected error in fixed recourse data
</commit_message>
<xml_diff>
--- a/Multiknapsack/results/fixed_recourse/multicut/M100_N200_T0_a25_ccg.xlsx
+++ b/Multiknapsack/results/fixed_recourse/multicut/M100_N200_T0_a25_ccg.xlsx
@@ -471,10 +471,10 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>-1438.4566348142198</v>
+        <v>-963.1075412558371</v>
       </c>
       <c r="C2">
-        <v>8.693624798</v>
+        <v>438.513680963</v>
       </c>
       <c r="D2">
         <v>2</v>
@@ -483,16 +483,16 @@
         <v>14</v>
       </c>
       <c r="F2">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="G2">
-        <v>1302</v>
+        <v>110400</v>
       </c>
       <c r="H2">
-        <v>1205</v>
+        <v>120500</v>
       </c>
       <c r="I2">
-        <v>100</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -500,10 +500,10 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>-1427.9132751704965</v>
+        <v>-960.465247165562</v>
       </c>
       <c r="C3">
-        <v>0.461959817</v>
+        <v>406.883121483</v>
       </c>
       <c r="D3">
         <v>2</v>
@@ -512,16 +512,16 @@
         <v>14</v>
       </c>
       <c r="F3">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="G3">
-        <v>1302</v>
+        <v>110400</v>
       </c>
       <c r="H3">
-        <v>1205</v>
+        <v>120500</v>
       </c>
       <c r="I3">
-        <v>100</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -529,10 +529,10 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>-1431.1234567604338</v>
+        <v>-962.1299820331453</v>
       </c>
       <c r="C4">
-        <v>0.411502318</v>
+        <v>1148.367505049</v>
       </c>
       <c r="D4">
         <v>2</v>
@@ -541,16 +541,16 @@
         <v>14</v>
       </c>
       <c r="F4">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="G4">
-        <v>1302</v>
+        <v>110400</v>
       </c>
       <c r="H4">
-        <v>1205</v>
+        <v>120500</v>
       </c>
       <c r="I4">
-        <v>100</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -558,10 +558,10 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>-1428.8271505904509</v>
+        <v>-958.1263449022533</v>
       </c>
       <c r="C5">
-        <v>0.388302154</v>
+        <v>831.356580329</v>
       </c>
       <c r="D5">
         <v>2</v>
@@ -570,16 +570,16 @@
         <v>14</v>
       </c>
       <c r="F5">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="G5">
-        <v>1302</v>
+        <v>110400</v>
       </c>
       <c r="H5">
-        <v>1205</v>
+        <v>120500</v>
       </c>
       <c r="I5">
-        <v>100</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -587,10 +587,10 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>-1430.8057250884558</v>
+        <v>-963.1399746398824</v>
       </c>
       <c r="C6">
-        <v>0.362502875</v>
+        <v>1021.811989351</v>
       </c>
       <c r="D6">
         <v>2</v>
@@ -599,16 +599,16 @@
         <v>14</v>
       </c>
       <c r="F6">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="G6">
-        <v>1302</v>
+        <v>110400</v>
       </c>
       <c r="H6">
-        <v>1205</v>
+        <v>120500</v>
       </c>
       <c r="I6">
-        <v>100</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -616,10 +616,10 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>-1422.6600489256507</v>
+        <v>-953.069846438852</v>
       </c>
       <c r="C7">
-        <v>0.306756942</v>
+        <v>516.375281886</v>
       </c>
       <c r="D7">
         <v>2</v>
@@ -628,16 +628,16 @@
         <v>14</v>
       </c>
       <c r="F7">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="G7">
-        <v>1302</v>
+        <v>110400</v>
       </c>
       <c r="H7">
-        <v>1205</v>
+        <v>120500</v>
       </c>
       <c r="I7">
-        <v>100</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -645,10 +645,10 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>-1434.332854599697</v>
+        <v>-965.4153674106826</v>
       </c>
       <c r="C8">
-        <v>0.262387791</v>
+        <v>954.205450714</v>
       </c>
       <c r="D8">
         <v>2</v>
@@ -657,16 +657,16 @@
         <v>14</v>
       </c>
       <c r="F8">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="G8">
-        <v>1302</v>
+        <v>110400</v>
       </c>
       <c r="H8">
-        <v>1205</v>
+        <v>120500</v>
       </c>
       <c r="I8">
-        <v>100</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -674,10 +674,10 @@
         <v>8</v>
       </c>
       <c r="B9">
-        <v>-1423.696623527594</v>
+        <v>-954.6051029237938</v>
       </c>
       <c r="C9">
-        <v>0.325357615</v>
+        <v>1215.461226395</v>
       </c>
       <c r="D9">
         <v>2</v>
@@ -686,16 +686,16 @@
         <v>14</v>
       </c>
       <c r="F9">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="G9">
-        <v>1302</v>
+        <v>110400</v>
       </c>
       <c r="H9">
-        <v>1205</v>
+        <v>120500</v>
       </c>
       <c r="I9">
-        <v>100</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -703,10 +703,10 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <v>-1430.5223557418108</v>
+        <v>-960.9871769768399</v>
       </c>
       <c r="C10">
-        <v>0.276595736</v>
+        <v>422.440112962</v>
       </c>
       <c r="D10">
         <v>2</v>
@@ -715,16 +715,16 @@
         <v>14</v>
       </c>
       <c r="F10">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="G10">
-        <v>1302</v>
+        <v>110400</v>
       </c>
       <c r="H10">
-        <v>1205</v>
+        <v>120500</v>
       </c>
       <c r="I10">
-        <v>100</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -732,10 +732,10 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>-1437.9375322645535</v>
+        <v>-965.36122253593</v>
       </c>
       <c r="C11">
-        <v>0.284815569</v>
+        <v>953.306023174</v>
       </c>
       <c r="D11">
         <v>2</v>
@@ -744,16 +744,16 @@
         <v>14</v>
       </c>
       <c r="F11">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="G11">
-        <v>1302</v>
+        <v>110400</v>
       </c>
       <c r="H11">
-        <v>1205</v>
+        <v>120500</v>
       </c>
       <c r="I11">
-        <v>100</v>
+        <v>10000</v>
       </c>
     </row>
   </sheetData>
@@ -797,10 +797,10 @@
         <v>0.0</v>
       </c>
       <c r="D2">
-        <v>0.06356561514404296</v>
+        <v>0.06519662681298828</v>
       </c>
       <c r="E2">
-        <v>78.64418</v>
+        <v>138.57865</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -808,13 +808,13 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>-1430.5223557418108</v>
+        <v>-960.9871769768399</v>
       </c>
       <c r="C3">
-        <v>0.0</v>
+        <v>0.004023830828155816</v>
       </c>
       <c r="D3">
-        <v>0.09844322250427245</v>
+        <v>416.2713530777032</v>
       </c>
       <c r="E3">
         <v>0.0</v>
@@ -861,10 +861,10 @@
         <v>0.0</v>
       </c>
       <c r="D2">
-        <v>0.06685417505004883</v>
+        <v>0.11287795769885253</v>
       </c>
       <c r="E2">
-        <v>72.37242</v>
+        <v>134.74132</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -872,13 +872,13 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>-1437.9375322645535</v>
+        <v>-965.36122253593</v>
       </c>
       <c r="C3">
-        <v>1.5812486310523797e-14</v>
+        <v>0.08386240805235516</v>
       </c>
       <c r="D3">
-        <v>0.10233816730957031</v>
+        <v>946.3168402140044</v>
       </c>
       <c r="E3">
         <v>0.0</v>
@@ -925,10 +925,10 @@
         <v>0.0</v>
       </c>
       <c r="D2">
-        <v>1.0213430298840331</v>
+        <v>0.8462853815408935</v>
       </c>
       <c r="E2">
-        <v>73.55054</v>
+        <v>136.22463</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -936,13 +936,13 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>-1438.4566348142198</v>
+        <v>-963.1075412558371</v>
       </c>
       <c r="C3">
-        <v>3.161355996979111e-14</v>
+        <v>0.002352205422191391</v>
       </c>
       <c r="D3">
-        <v>0.2619510062053223</v>
+        <v>425.3277832817665</v>
       </c>
       <c r="E3">
         <v>0.0</v>
@@ -989,10 +989,10 @@
         <v>0.0</v>
       </c>
       <c r="D2">
-        <v>0.12030756274182129</v>
+        <v>0.07757260252770996</v>
       </c>
       <c r="E2">
-        <v>74.36795</v>
+        <v>137.1635</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -1000,13 +1000,13 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>-1427.9132751704965</v>
+        <v>-960.465247165562</v>
       </c>
       <c r="C3">
-        <v>1.5923493351938137e-14</v>
+        <v>0.0008404312086639922</v>
       </c>
       <c r="D3">
-        <v>0.14797390750354003</v>
+        <v>400.785045977442</v>
       </c>
       <c r="E3">
         <v>0.0</v>
@@ -1053,10 +1053,10 @@
         <v>0.0</v>
       </c>
       <c r="D2">
-        <v>0.08155222138012695</v>
+        <v>0.13341643966540528</v>
       </c>
       <c r="E2">
-        <v>74.35989</v>
+        <v>136.59474</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -1064,13 +1064,13 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>-1431.1234567604338</v>
+        <v>-962.1299820331453</v>
       </c>
       <c r="C3">
-        <v>0.0</v>
+        <v>0.05491416457396366</v>
       </c>
       <c r="D3">
-        <v>0.1365046438601074</v>
+        <v>1142.279286326067</v>
       </c>
       <c r="E3">
         <v>0.0</v>
@@ -1117,10 +1117,10 @@
         <v>0.0</v>
       </c>
       <c r="D2">
-        <v>0.08816138122827148</v>
+        <v>0.10627470621508789</v>
       </c>
       <c r="E2">
-        <v>76.03954</v>
+        <v>137.84913</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -1128,13 +1128,13 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>-1428.8271505904509</v>
+        <v>-958.1263449022533</v>
       </c>
       <c r="C3">
-        <v>4.773992613786542e-14</v>
+        <v>0.09879981259225552</v>
       </c>
       <c r="D3">
-        <v>0.1346705185352783</v>
+        <v>824.6910076974402</v>
       </c>
       <c r="E3">
         <v>0.0</v>
@@ -1181,10 +1181,10 @@
         <v>0.0</v>
       </c>
       <c r="D2">
-        <v>0.07699399367089843</v>
+        <v>0.08166881313964844</v>
       </c>
       <c r="E2">
-        <v>69.71563</v>
+        <v>138.89541</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -1192,13 +1192,13 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>-1430.8057250884558</v>
+        <v>-963.1399746398824</v>
       </c>
       <c r="C3">
-        <v>0.0</v>
+        <v>0.09222430419959636</v>
       </c>
       <c r="D3">
-        <v>0.1364052211767578</v>
+        <v>1016.0596363792858</v>
       </c>
       <c r="E3">
         <v>0.0</v>
@@ -1245,10 +1245,10 @@
         <v>0.0</v>
       </c>
       <c r="D2">
-        <v>0.08393977685437012</v>
+        <v>0.11606455872436523</v>
       </c>
       <c r="E2">
-        <v>78.2729</v>
+        <v>136.79724</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -1256,13 +1256,13 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>-1422.6600489256507</v>
+        <v>-953.069846438852</v>
       </c>
       <c r="C3">
         <v>0.0</v>
       </c>
       <c r="D3">
-        <v>0.10919170410571288</v>
+        <v>510.0949633082174</v>
       </c>
       <c r="E3">
         <v>0.0</v>
@@ -1309,10 +1309,10 @@
         <v>0.0</v>
       </c>
       <c r="D2">
-        <v>0.04706580867419433</v>
+        <v>0.10300813076916504</v>
       </c>
       <c r="E2">
-        <v>70.82809</v>
+        <v>136.77823</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -1320,13 +1320,13 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>-1434.332854599697</v>
+        <v>-965.4153674106826</v>
       </c>
       <c r="C3">
-        <v>0.0</v>
+        <v>0.006156580694377443</v>
       </c>
       <c r="D3">
-        <v>0.12237100392407227</v>
+        <v>947.7586012058363</v>
       </c>
       <c r="E3">
         <v>0.0</v>
@@ -1373,10 +1373,10 @@
         <v>0.0</v>
       </c>
       <c r="D2">
-        <v>0.06278242747412109</v>
+        <v>0.11353465360314942</v>
       </c>
       <c r="E2">
-        <v>73.47673</v>
+        <v>139.2123</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -1384,13 +1384,13 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>-1423.696623527594</v>
+        <v>-954.6051029237938</v>
       </c>
       <c r="C3">
-        <v>0.0</v>
+        <v>0.029341303106506938</v>
       </c>
       <c r="D3">
-        <v>0.12904563101245117</v>
+        <v>1209.368990072879</v>
       </c>
       <c r="E3">
         <v>0.0</v>

</xml_diff>